<commit_message>
further ajustments 2, plus nice plots
</commit_message>
<xml_diff>
--- a/case study propionate/results_v2.xlsx
+++ b/case study propionate/results_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\case study propionate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A33B6FD-7BEF-43FC-8C05-211F7A29A662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3983806D-FBCE-4904-8B1D-1371C70799CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2375,20 +2375,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.1796875" customWidth="1"/>
+    <col min="1" max="1" width="34.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>15.681000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>705.6450000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>32.683007501547472</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>32.783007501547473</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>298.90680228772959</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>64.639264533585845</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>15.280640000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2906,7 +2906,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -3151,7 +3151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>52</v>
       </c>

</xml_diff>